<commit_message>
Stats page - fixed percentage, added some stats, added rounding
</commit_message>
<xml_diff>
--- a/Designs/Work Items Master.xlsx
+++ b/Designs/Work Items Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_MyWork\Source\DominosPizzaPicker\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841D32CB-BBC8-4EF1-88B7-D1291C0B313D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D3813F-945A-456A-B1E2-5E8C56614D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5100" windowWidth="29040" windowHeight="15840" xr2:uid="{485CD9D7-478E-4053-8A03-E6F690CA9E6D}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Item</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>various other changes</t>
+  </si>
+  <si>
+    <t>Added a pretty bare bones page. All it has is number of pizzas eaten of total, but it's there</t>
+  </si>
+  <si>
+    <t>39f81aa8</t>
   </si>
 </sst>
 </file>
@@ -537,8 +543,8 @@
   <dimension ref="A1:F874"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,19 +729,25 @@
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="5">
+        <v>44453</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">

</xml_diff>